<commit_message>
cap nhat sau buoi review a Manh
</commit_message>
<xml_diff>
--- a/Danh_sach_can_bo.xlsx
+++ b/Danh_sach_can_bo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEGION\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MisaFresher\misa.qlth.frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -156,42 +156,6 @@
     <t>Dang_lam_viec</t>
   </si>
   <si>
-    <t>Terence Oneal</t>
-  </si>
-  <si>
-    <t>Ardelia Stowe</t>
-  </si>
-  <si>
-    <t>Lavonne Her</t>
-  </si>
-  <si>
-    <t>Vita Aguirre</t>
-  </si>
-  <si>
-    <t>Marty Covington</t>
-  </si>
-  <si>
-    <t>Luna Britton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oneal Terence </t>
-  </si>
-  <si>
-    <t>Stowe Ardelia</t>
-  </si>
-  <si>
-    <t>Her Lavonne</t>
-  </si>
-  <si>
-    <t>Aguirre Vita</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Covington Marty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Britton Luna </t>
-  </si>
-  <si>
     <t>1230</t>
   </si>
   <si>
@@ -202,6 +166,42 @@
   </si>
   <si>
     <t>MS215</t>
+  </si>
+  <si>
+    <t>Nguyễn Trung Trực</t>
+  </si>
+  <si>
+    <t>Đặng Anh Tuấn</t>
+  </si>
+  <si>
+    <t>Đặng Thu Thảo</t>
+  </si>
+  <si>
+    <t>Hoàng Nguyệt Anh</t>
+  </si>
+  <si>
+    <t>Công Tôn Sách</t>
+  </si>
+  <si>
+    <t>Trương Phi</t>
+  </si>
+  <si>
+    <t>Quan Vân Trường</t>
+  </si>
+  <si>
+    <t>Lưu Bị</t>
+  </si>
+  <si>
+    <t>Thủy Kính</t>
+  </si>
+  <si>
+    <t>Xích Thố</t>
+  </si>
+  <si>
+    <t>Hoàng Linh Mai</t>
+  </si>
+  <si>
+    <t>Tiểu Kiều</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,13 +641,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
@@ -669,10 +669,10 @@
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -698,7 +698,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
@@ -725,10 +725,10 @@
         <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>4</v>
@@ -750,7 +750,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
@@ -773,7 +773,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -802,7 +802,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>11</v>
@@ -831,7 +831,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
@@ -856,7 +856,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>16</v>
@@ -885,7 +885,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>19</v>
@@ -912,7 +912,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
@@ -937,7 +937,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>23</v>

</xml_diff>